<commit_message>
committing from Devireddy - kalyankar
</commit_message>
<xml_diff>
--- a/Gadge_LabExam03Grading.xlsx
+++ b/Gadge_LabExam03Grading.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533574\Desktop\44542 Spring 2019\Lab Exams\Lab Exam 03\LabExam3Rubrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LabExam3Rubrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>Author notation</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>(-2.5) for getting UnsupportedOperationException while running driver class</t>
+  </si>
+  <si>
+    <t>(-8) For not writing logic/implementation.</t>
   </si>
 </sst>
 </file>
@@ -423,6 +426,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,18 +448,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1523,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,14 +1541,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1634,11 +1637,11 @@
       <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="6">
         <f>SUM(D3:D6)</f>
         <v>7</v>
@@ -1650,14 +1653,14 @@
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -1762,11 +1765,11 @@
       <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="6">
         <f>SUM(D10:D14)</f>
         <v>10</v>
@@ -1778,14 +1781,14 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
@@ -1860,7 +1863,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1960,11 +1963,11 @@
       <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="6">
         <f>SUM(D18:D25)</f>
         <v>56</v>
@@ -1976,14 +1979,14 @@
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
@@ -2046,11 +2049,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="6">
         <f>SUM(D29:D30)</f>
         <v>20</v>
@@ -2062,14 +2065,14 @@
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
@@ -2112,11 +2115,11 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="6">
         <f>SUM(D34:D34)</f>
         <v>7</v>
@@ -2128,14 +2131,14 @@
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="28"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
@@ -2158,11 +2161,11 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="10">
         <f>SUM(D7, D15, D26, D35, D31)</f>
         <v>100</v>
@@ -2175,11 +2178,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A35:C35"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A16:F16"/>
@@ -2187,6 +2185,11 @@
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A32:F32"/>
     <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>